<commit_message>
3V3 boost converter replacement
</commit_message>
<xml_diff>
--- a/Cost breakdown.xlsx
+++ b/Cost breakdown.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\DIY\Ordinateur de bord Parapente\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="149">
   <si>
     <t>Part</t>
   </si>
@@ -479,7 +474,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -526,7 +521,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -543,7 +538,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
@@ -768,6 +763,132 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -787,15 +908,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -814,139 +926,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -962,38 +957,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S52" totalsRowCount="1" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S52" totalsRowCount="1" headerRowDxfId="38">
   <autoFilter ref="A1:S51"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="Part" totalsRowLabel="Total" dataDxfId="38" totalsRowDxfId="18"/>
-    <tableColumn id="2" name="Value" dataDxfId="37" totalsRowDxfId="17"/>
-    <tableColumn id="3" name="Package" dataDxfId="36" totalsRowDxfId="16"/>
-    <tableColumn id="4" name="Qty" dataDxfId="35" totalsRowDxfId="15"/>
-    <tableColumn id="5" name="Farnell part num" dataDxfId="34" totalsRowDxfId="14"/>
-    <tableColumn id="6" name="Prix Farnell" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="13" dataCellStyle="Currency"/>
-    <tableColumn id="19" name="Farnell TTC" dataDxfId="20" totalsRowDxfId="12" dataCellStyle="Currency">
+    <tableColumn id="1" name="Part" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="18"/>
+    <tableColumn id="2" name="Value" dataDxfId="36" totalsRowDxfId="17"/>
+    <tableColumn id="3" name="Package" dataDxfId="35" totalsRowDxfId="16"/>
+    <tableColumn id="4" name="Qty" dataDxfId="34" totalsRowDxfId="15"/>
+    <tableColumn id="5" name="Farnell part num" dataDxfId="33" totalsRowDxfId="14"/>
+    <tableColumn id="6" name="Prix Farnell" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="13"/>
+    <tableColumn id="19" name="Farnell TTC" dataDxfId="31" totalsRowDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Prix Farnell]]*1.196</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Digikey part num" dataDxfId="32" totalsRowDxfId="11"/>
-    <tableColumn id="8" name="Prix Digikey" dataDxfId="31" totalsRowDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="9" name="en EUR" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="9" dataCellStyle="Currency">
+    <tableColumn id="7" name="Digikey part num" dataDxfId="30" totalsRowDxfId="11"/>
+    <tableColumn id="8" name="Prix Digikey" dataDxfId="29" totalsRowDxfId="10"/>
+    <tableColumn id="9" name="en EUR" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="9">
       <calculatedColumnFormula>(I2/1.28627)*1.196</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="SparkFun part num" dataDxfId="29" totalsRowDxfId="8"/>
-    <tableColumn id="11" name="Prix Sparkfun" dataDxfId="28" totalsRowDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="12" name="en EUR2" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="10" name="SparkFun part num" dataDxfId="27" totalsRowDxfId="8"/>
+    <tableColumn id="11" name="Prix Sparkfun" dataDxfId="26" totalsRowDxfId="7"/>
+    <tableColumn id="12" name="en EUR2" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="6">
       <calculatedColumnFormula>(L2/1.28627)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Adafruit part num" dataDxfId="26" totalsRowDxfId="5"/>
-    <tableColumn id="14" name="Prix Adafruit" dataDxfId="25" totalsRowDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="15" name="en EUR3" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="13" name="Adafruit part num" dataDxfId="24" totalsRowDxfId="5"/>
+    <tableColumn id="14" name="Prix Adafruit" dataDxfId="23" totalsRowDxfId="4"/>
+    <tableColumn id="15" name="en EUR3" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="3">
       <calculatedColumnFormula>(O2/1.28627)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Choix fournisseur" dataDxfId="23" totalsRowDxfId="2"/>
-    <tableColumn id="17" name="Réf fournisseur" dataDxfId="22" totalsRowDxfId="1">
+    <tableColumn id="16" name="Choix fournisseur" dataDxfId="21" totalsRowDxfId="2"/>
+    <tableColumn id="17" name="Réf fournisseur" dataDxfId="20" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Q2="Farnell",E2,IF(Q2="Digikey",H2,IF(Q2="Sparkfun",K2,IF(Q2="Adafruit",N2,"N/A"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Prix fournisseur" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="18" name="Prix fournisseur" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Choix fournisseur]]="Farnell",Table1[[#This Row],[Farnell TTC]],IF(Table1[[#This Row],[Choix fournisseur]]="Digikey",Table1[[#This Row],[en EUR]],IF(Table1[[#This Row],[Choix fournisseur]]="Sparkfun",Table1[[#This Row],[en EUR2]],IF(Table1[[#This Row],[Choix fournisseur]]="Adafruit",Table1[[#This Row],[en EUR3]],0))))*Table1[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1044,7 +1039,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -1079,7 +1074,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -1256,7 +1251,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1266,20 +1261,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.28515625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
     <col min="9" max="10" width="9.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
@@ -2189,10 +2185,15 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="E21" s="1">
+        <v>1515662</v>
+      </c>
+      <c r="F21" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
       <c r="G21" s="2">
         <f>Table1[[#This Row],[Prix Farnell]]*1.196</f>
-        <v>0</v>
+        <v>0.11003199999999999</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="2">
@@ -2209,13 +2210,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
+      <c r="Q21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="3"/>
+        <v>1515662</v>
       </c>
       <c r="S21" s="2">
         <f>IF(Table1[[#This Row],[Choix fournisseur]]="Farnell",Table1[[#This Row],[Farnell TTC]],IF(Table1[[#This Row],[Choix fournisseur]]="Digikey",Table1[[#This Row],[en EUR]],IF(Table1[[#This Row],[Choix fournisseur]]="Sparkfun",Table1[[#This Row],[en EUR2]],IF(Table1[[#This Row],[Choix fournisseur]]="Adafruit",Table1[[#This Row],[en EUR3]],0))))*Table1[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.11003199999999999</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -2231,10 +2235,15 @@
       <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="E22" s="1">
+        <v>2118126</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.26</v>
+      </c>
       <c r="G22" s="2">
         <f>Table1[[#This Row],[Prix Farnell]]*1.196</f>
-        <v>0</v>
+        <v>0.31096000000000001</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="2">
@@ -2251,13 +2260,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
+      <c r="Q22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="3"/>
+        <v>2118126</v>
       </c>
       <c r="S22" s="2">
         <f>IF(Table1[[#This Row],[Choix fournisseur]]="Farnell",Table1[[#This Row],[Farnell TTC]],IF(Table1[[#This Row],[Choix fournisseur]]="Digikey",Table1[[#This Row],[en EUR]],IF(Table1[[#This Row],[Choix fournisseur]]="Sparkfun",Table1[[#This Row],[en EUR2]],IF(Table1[[#This Row],[Choix fournisseur]]="Adafruit",Table1[[#This Row],[en EUR3]],0))))*Table1[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.62192000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -3612,7 +3624,7 @@
       </c>
       <c r="F52" s="6">
         <f>SUBTOTAL(109,Table1[Prix Farnell])</f>
-        <v>118.57</v>
+        <v>118.922</v>
       </c>
       <c r="G52" s="6"/>
       <c r="I52" s="5"/>
@@ -3632,7 +3644,7 @@
       </c>
       <c r="S52" s="6">
         <f>SUBTOTAL(109,Table1[Prix fournisseur])</f>
-        <v>179.02814617086611</v>
+        <v>179.76009817086612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>